<commit_message>
add new calculation and method
</commit_message>
<xml_diff>
--- a/Datas/data_description.xlsx
+++ b/Datas/data_description.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,45 +436,30 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>random kmeans</t>
+          <t>kmeans++</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>kde kmeans</t>
+          <t>random SOM</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>kmeans++</t>
+          <t>kmeans SOM</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>random SOM</t>
+          <t>kmeans++ SOM</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>kmeans SOM</t>
+          <t>SOM++</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>kde kmeans SOM</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>kmeans++ SOM</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>SOM++</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>kde SOM</t>
         </is>
@@ -487,31 +472,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C2" t="n">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="D2" t="n">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E2" t="n">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F2" t="n">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="G2" t="n">
-        <v>61</v>
-      </c>
-      <c r="H2" t="n">
-        <v>61</v>
-      </c>
-      <c r="I2" t="n">
-        <v>61</v>
-      </c>
-      <c r="J2" t="n">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
@@ -521,31 +497,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.8192</v>
+        <v>0.2934</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8135</v>
+        <v>0.2847</v>
       </c>
       <c r="D3" t="n">
-        <v>0.618</v>
+        <v>-1</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6935</v>
+        <v>0.4207</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7015</v>
+        <v>0.3586</v>
       </c>
       <c r="G3" t="n">
-        <v>0.6778</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.6218</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.6191</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.7395</v>
+        <v>0.4707</v>
       </c>
     </row>
     <row r="4">
@@ -555,31 +522,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.0107</v>
+        <v>0.0598</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0106</v>
+        <v>0.2466</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0532</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2057</v>
+        <v>0.3431</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2148</v>
+        <v>0.143</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2245</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.1758</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.0997</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.172</v>
+        <v>0.0985</v>
       </c>
     </row>
     <row r="5">
@@ -589,31 +547,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.8007</v>
+        <v>0.2304</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7615</v>
+        <v>-0.3911</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5224</v>
+        <v>-1</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0004</v>
+        <v>-1</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.1721</v>
+        <v>0.1212</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0584</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.2556</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.3994</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.2012</v>
+        <v>0.2442</v>
       </c>
     </row>
     <row r="6">
@@ -623,31 +572,22 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.8122</v>
+        <v>0.2639</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8066</v>
+        <v>0.1191</v>
       </c>
       <c r="D6" t="n">
-        <v>0.5498</v>
+        <v>-1</v>
       </c>
       <c r="E6" t="n">
-        <v>0.6367</v>
+        <v>0.2919</v>
       </c>
       <c r="F6" t="n">
-        <v>0.634</v>
+        <v>0.2621</v>
       </c>
       <c r="G6" t="n">
-        <v>0.6424</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.4675</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.5367</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.72</v>
+        <v>0.397</v>
       </c>
     </row>
     <row r="7">
@@ -657,31 +597,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.8142</v>
+        <v>0.2772</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8131</v>
+        <v>0.3326</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6462</v>
+        <v>-1</v>
       </c>
       <c r="E7" t="n">
-        <v>0.7742</v>
+        <v>0.4218</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8064</v>
+        <v>0.3472</v>
       </c>
       <c r="G7" t="n">
-        <v>0.7933</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.6706</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.655</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.8047</v>
+        <v>0.4317</v>
       </c>
     </row>
     <row r="8">
@@ -691,31 +622,22 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.8327</v>
+        <v>0.2907</v>
       </c>
       <c r="C8" t="n">
-        <v>0.8148</v>
+        <v>0.42</v>
       </c>
       <c r="D8" t="n">
-        <v>0.6592</v>
+        <v>-1</v>
       </c>
       <c r="E8" t="n">
-        <v>0.8358</v>
+        <v>0.6521</v>
       </c>
       <c r="F8" t="n">
-        <v>0.8358</v>
+        <v>0.4283</v>
       </c>
       <c r="G8" t="n">
-        <v>0.8339</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.7813</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.6757</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.8358</v>
+        <v>0.5809</v>
       </c>
     </row>
     <row r="9">
@@ -725,31 +647,22 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.8351</v>
+        <v>0.471</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8357</v>
+        <v>0.7929</v>
       </c>
       <c r="D9" t="n">
-        <v>0.6874</v>
+        <v>-1</v>
       </c>
       <c r="E9" t="n">
-        <v>0.8611</v>
+        <v>0.8189</v>
       </c>
       <c r="F9" t="n">
-        <v>0.8611</v>
+        <v>0.8189</v>
       </c>
       <c r="G9" t="n">
-        <v>0.8611</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.8358</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.7986</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0.8611</v>
+        <v>0.611</v>
       </c>
     </row>
   </sheetData>

</xml_diff>